<commit_message>
Change role base authorization
</commit_message>
<xml_diff>
--- a/demo/generated-reports/Financial_Report_2025.xlsx
+++ b/demo/generated-reports/Financial_Report_2025.xlsx
@@ -38,7 +38,7 @@
     <t>Spending</t>
   </si>
   <si>
-    <t>2025-03-06</t>
+    <t>2025-03-18</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>200.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="4">
@@ -152,7 +152,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>200.0</v>
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>